<commit_message>
leds added, less nested while loop
</commit_message>
<xml_diff>
--- a/ttk8/diagrams/semester_wbs_plan.xlsx
+++ b/ttk8/diagrams/semester_wbs_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebekka/koding/ntnu/semesterprosjekt/arduino_camera/ttk8/diagrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366866F0-6441-B846-A7EE-EC5F8C9DDF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D70915-B456-5447-8813-E7CAB46DE9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1676,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="131" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1860,11 +1860,11 @@
       </c>
       <c r="C10" s="69">
         <f>SUM(F43,F40,F37,F34,F31,F24,F20,F17,F14,F27)</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="70">
         <f>AVERAGE(G43,G40,G37,G34,G31,G24,G20,G17,G14,G27)</f>
-        <v>0.42666666666666664</v>
+        <v>0.4291666666666667</v>
       </c>
       <c r="E10" s="72" t="s">
         <v>68</v>
@@ -2566,11 +2566,11 @@
       </c>
       <c r="F31" s="12">
         <f>SUM(F32:F33)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G31" s="91">
         <f>AVERAGE(G32:G33)</f>
-        <v>0.15</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="H31" s="105"/>
       <c r="I31" s="105"/>
@@ -2633,14 +2633,16 @@
       </c>
       <c r="F33" s="15">
         <f>SUM(H33:P33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="96">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H33" s="105"/>
       <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="J33" s="38">
+        <v>1</v>
+      </c>
       <c r="K33" s="39"/>
       <c r="L33" s="36"/>
       <c r="M33" s="36"/>

</xml_diff>